<commit_message>
Timeline + Variablen verteilt
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loure\Desktop\Master Business Analytics and Econometrics\Semester 3\Bayesian Analytics\Replication challenge\Replication-Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2271DDBA-A5AD-488E-B156-28ABD511FD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FED0B90-E89D-498D-8CD4-30B98761436E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>20.11.2025 - 27.11.2025</t>
   </si>
@@ -90,12 +90,6 @@
     <t>Paper lesen</t>
   </si>
   <si>
-    <t>EDA</t>
-  </si>
-  <si>
-    <t>Summary statistics</t>
-  </si>
-  <si>
     <t>Variablen Aufteilen</t>
   </si>
   <si>
@@ -106,6 +100,15 @@
   </si>
   <si>
     <t>model evaluation WAIC etc.</t>
+  </si>
+  <si>
+    <t>EDA(DAGs)</t>
+  </si>
+  <si>
+    <t>Summary statistics(Latex style) Nico</t>
+  </si>
+  <si>
+    <t>EDA(correlation heatmap) Lourenco</t>
   </si>
 </sst>
 </file>
@@ -160,15 +163,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -458,7 +460,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.19921875" bestFit="1" customWidth="1"/>
@@ -502,44 +504,39 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">

</xml_diff>